<commit_message>
edits for gbirg slides
</commit_message>
<xml_diff>
--- a/DAVID/E2F.DAVID.xlsx
+++ b/DAVID/E2F.DAVID.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\ABRF_GBIRG_OntologyStudy\DAVID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{42FB1C2A-415E-4CFD-B772-25B8E0551CAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBB9732-B115-4ABB-874F-D131B623D110}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22755" windowHeight="11235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22755" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E2F.DAVID" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'E2F.DAVID'!$A$1:$N$543</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -3112,7 +3115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3947,11 +3950,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N543"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109:XFD109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4004,7 +4008,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -4048,7 +4052,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -4092,7 +4096,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>179</v>
       </c>
@@ -4136,7 +4140,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>235</v>
       </c>
@@ -4180,7 +4184,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>247</v>
       </c>
@@ -4224,7 +4228,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>274</v>
       </c>
@@ -4268,7 +4272,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>314</v>
       </c>
@@ -4312,7 +4316,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>349</v>
       </c>
@@ -4356,7 +4360,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>510</v>
       </c>
@@ -4400,7 +4404,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>569</v>
       </c>
@@ -4884,7 +4888,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -4928,7 +4932,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -4972,7 +4976,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -5016,7 +5020,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -5060,7 +5064,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -5104,7 +5108,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -5148,7 +5152,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>125</v>
       </c>
@@ -5192,7 +5196,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -5236,7 +5240,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -5280,7 +5284,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -5324,7 +5328,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -5368,7 +5372,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -5412,7 +5416,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -5456,7 +5460,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -5500,7 +5504,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -5544,7 +5548,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -5588,7 +5592,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>149</v>
       </c>
@@ -5632,7 +5636,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>181</v>
       </c>
@@ -5676,7 +5680,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>216</v>
       </c>
@@ -5720,7 +5724,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>225</v>
       </c>
@@ -5764,7 +5768,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -5808,7 +5812,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -5852,7 +5856,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -5896,7 +5900,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>106</v>
       </c>
@@ -5940,7 +5944,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>111</v>
       </c>
@@ -5984,7 +5988,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>145</v>
       </c>
@@ -6028,7 +6032,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>159</v>
       </c>
@@ -6072,7 +6076,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>190</v>
       </c>
@@ -6116,7 +6120,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>193</v>
       </c>
@@ -6160,7 +6164,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>214</v>
       </c>
@@ -6204,7 +6208,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>36</v>
       </c>
@@ -6248,7 +6252,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>40</v>
       </c>
@@ -6292,7 +6296,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>44</v>
       </c>
@@ -6336,7 +6340,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -6380,7 +6384,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -6424,7 +6428,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -6468,7 +6472,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -6512,7 +6516,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -6556,7 +6560,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -6600,7 +6604,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -6644,7 +6648,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>571</v>
       </c>
@@ -6685,7 +6689,7 @@
         <v>2.9155552056613598</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>609</v>
       </c>
@@ -6726,7 +6730,7 @@
         <v>4.8000896869163103</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>669</v>
       </c>
@@ -6767,7 +6771,7 @@
         <v>7.3905713802252402</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>749</v>
       </c>
@@ -6808,7 +6812,7 @@
         <v>12.243541454218599</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>903</v>
       </c>
@@ -6849,7 +6853,7 @@
         <v>23.718245850253901</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>937</v>
       </c>
@@ -6890,7 +6894,7 @@
         <v>23.718245850253901</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>950</v>
       </c>
@@ -6931,7 +6935,7 @@
         <v>23.718245850253901</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>952</v>
       </c>
@@ -16074,7 +16078,7 @@
         <v>37.666128305510703</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>175</v>
       </c>
@@ -16115,7 +16119,7 @@
         <v>2.35865479620609E-5</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>177</v>
       </c>
@@ -16156,7 +16160,7 @@
         <v>2.4474159810423199E-5</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>195</v>
       </c>
@@ -16197,7 +16201,7 @@
         <v>1.8947939017931799E-4</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>198</v>
       </c>
@@ -16238,7 +16242,7 @@
         <v>2.3021700288198801E-4</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>206</v>
       </c>
@@ -16279,7 +16283,7 @@
         <v>6.6731738150357098E-4</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>218</v>
       </c>
@@ -16320,7 +16324,7 @@
         <v>9.6715133721605605E-4</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>221</v>
       </c>
@@ -16361,7 +16365,7 @@
         <v>1.30232737469888E-3</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>229</v>
       </c>
@@ -16402,7 +16406,7 @@
         <v>1.4750330763754901E-3</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>249</v>
       </c>
@@ -16443,7 +16447,7 @@
         <v>4.5611627913237597E-3</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>260</v>
       </c>
@@ -16484,7 +16488,7 @@
         <v>6.6284329155010101E-3</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>270</v>
       </c>
@@ -16525,7 +16529,7 @@
         <v>1.1508191422321601E-2</v>
       </c>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>276</v>
       </c>
@@ -16566,7 +16570,7 @@
         <v>1.4282341087039199E-2</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>288</v>
       </c>
@@ -16607,7 +16611,7 @@
         <v>2.08533559877952E-2</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>294</v>
       </c>
@@ -16648,7 +16652,7 @@
         <v>2.6350695517385999E-2</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>296</v>
       </c>
@@ -16689,7 +16693,7 @@
         <v>2.6800658328030101E-2</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>302</v>
       </c>
@@ -16730,7 +16734,7 @@
         <v>3.0406125795987501E-2</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>310</v>
       </c>
@@ -16771,7 +16775,7 @@
         <v>3.7916729383147101E-2</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>322</v>
       </c>
@@ -16812,7 +16816,7 @@
         <v>5.8558538417318798E-2</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>332</v>
       </c>
@@ -16853,7 +16857,7 @@
         <v>7.2615940321523506E-2</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>334</v>
       </c>
@@ -16894,7 +16898,7 @@
         <v>7.6809301851767695E-2</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>338</v>
       </c>
@@ -16935,7 +16939,7 @@
         <v>8.6570948369610795E-2</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>347</v>
       </c>
@@ -16976,7 +16980,7 @@
         <v>0.100243104340032</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>404</v>
       </c>
@@ -17017,7 +17021,7 @@
         <v>0.37623955654603303</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>410</v>
       </c>
@@ -17058,7 +17062,7 @@
         <v>0.41405154278020601</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>445</v>
       </c>
@@ -17099,7 +17103,7 @@
         <v>0.74883251563916797</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>451</v>
       </c>
@@ -17140,7 +17144,7 @@
         <v>0.78945676996304703</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>456</v>
       </c>
@@ -17181,7 +17185,7 @@
         <v>0.839904182210091</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>464</v>
       </c>
@@ -17222,7 +17226,7 @@
         <v>0.86782238815156798</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>466</v>
       </c>
@@ -17263,7 +17267,7 @@
         <v>0.86782238815156798</v>
       </c>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>468</v>
       </c>
@@ -17304,7 +17308,7 @@
         <v>0.86782238815156798</v>
       </c>
     </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>504</v>
       </c>
@@ -17345,7 +17349,7 @@
         <v>1.17719256736037</v>
       </c>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>506</v>
       </c>
@@ -17386,7 +17390,7 @@
         <v>1.1785641775725799</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>528</v>
       </c>
@@ -17427,7 +17431,7 @@
         <v>1.44585481923305</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>530</v>
       </c>
@@ -17468,7 +17472,7 @@
         <v>1.45255443323725</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>539</v>
       </c>
@@ -17509,7 +17513,7 @@
         <v>1.8135708935413899</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>551</v>
       </c>
@@ -17550,7 +17554,7 @@
         <v>2.2025167797697298</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>565</v>
       </c>
@@ -17591,7 +17595,7 @@
         <v>2.5538500201319398</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>602</v>
       </c>
@@ -17632,7 +17636,7 @@
         <v>4.1530752598453997</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>611</v>
       </c>
@@ -17673,7 +17677,7 @@
         <v>4.6622487695880004</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>626</v>
       </c>
@@ -17714,7 +17718,7 @@
         <v>5.1861917755172202</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>644</v>
       </c>
@@ -17755,7 +17759,7 @@
         <v>5.7232629790086103</v>
       </c>
     </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>658</v>
       </c>
@@ -17796,7 +17800,7 @@
         <v>6.6434990488113401</v>
       </c>
     </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>686</v>
       </c>
@@ -17837,7 +17841,7 @@
         <v>7.7674635636402796</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>688</v>
       </c>
@@ -17878,7 +17882,7 @@
         <v>7.7814569673337299</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>694</v>
       </c>
@@ -17919,7 +17923,7 @@
         <v>8.0062603914515602</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>696</v>
       </c>
@@ -17960,7 +17964,7 @@
         <v>8.0062603914515602</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>698</v>
       </c>
@@ -18001,7 +18005,7 @@
         <v>8.0062603914515602</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>731</v>
       </c>
@@ -18042,7 +18046,7 @@
         <v>8.9876621590365495</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>751</v>
       </c>
@@ -18083,7 +18087,7 @@
         <v>11.1158350143394</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>755</v>
       </c>
@@ -18124,7 +18128,7 @@
         <v>11.3498578462687</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>787</v>
       </c>
@@ -18165,7 +18169,7 @@
         <v>12.342957825099001</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>793</v>
       </c>
@@ -18206,7 +18210,7 @@
         <v>13.464466134449401</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>801</v>
       </c>
@@ -18247,7 +18251,7 @@
         <v>13.896862207502201</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>802</v>
       </c>
@@ -18288,7 +18292,7 @@
         <v>13.896862207502201</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>804</v>
       </c>
@@ -18329,7 +18333,7 @@
         <v>13.896862207502201</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>853</v>
       </c>
@@ -18370,7 +18374,7 @@
         <v>16.519038278311299</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>855</v>
       </c>
@@ -18411,7 +18415,7 @@
         <v>16.519038278311299</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>857</v>
       </c>
@@ -18452,7 +18456,7 @@
         <v>16.519038278311299</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>895</v>
       </c>
@@ -18493,7 +18497,7 @@
         <v>18.887478090672101</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>896</v>
       </c>
@@ -18534,7 +18538,7 @@
         <v>18.887478090672101</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>897</v>
       </c>
@@ -18575,7 +18579,7 @@
         <v>18.887478090672101</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>939</v>
       </c>
@@ -18616,7 +18620,7 @@
         <v>20.752914923556599</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>941</v>
       </c>
@@ -18657,7 +18661,7 @@
         <v>20.752914923556599</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>943</v>
       </c>
@@ -18698,7 +18702,7 @@
         <v>20.752914923556599</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>944</v>
       </c>
@@ -18739,7 +18743,7 @@
         <v>20.752914923556599</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>954</v>
       </c>
@@ -18780,7 +18784,7 @@
         <v>21.400771947806199</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>958</v>
       </c>
@@ -18821,7 +18825,7 @@
         <v>21.491053326519701</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>973</v>
       </c>
@@ -18862,7 +18866,7 @@
         <v>22.121136712516002</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>975</v>
       </c>
@@ -18903,7 +18907,7 @@
         <v>22.121136712516002</v>
       </c>
     </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>977</v>
       </c>
@@ -18944,7 +18948,7 @@
         <v>22.121136712516002</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>1006</v>
       </c>
@@ -18985,7 +18989,7 @@
         <v>24.1548898515492</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>1007</v>
       </c>
@@ -19026,7 +19030,7 @@
         <v>24.1548898515492</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>1025</v>
       </c>
@@ -19067,7 +19071,7 @@
         <v>26.065732680077801</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>1027</v>
       </c>
@@ -19108,7 +19112,7 @@
         <v>26.065732680077801</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>231</v>
       </c>
@@ -19149,7 +19153,7 @@
         <v>3.23904645960437E-3</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>259</v>
       </c>
@@ -19190,7 +19194,7 @@
         <v>1.37586230766974E-2</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>290</v>
       </c>
@@ -19231,7 +19235,7 @@
         <v>4.9291702354299298E-2</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>316</v>
       </c>
@@ -19272,7 +19276,7 @@
         <v>0.102773478378323</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>318</v>
       </c>
@@ -19313,7 +19317,7 @@
         <v>0.13832589201030099</v>
       </c>
     </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>324</v>
       </c>
@@ -19354,7 +19358,7 @@
         <v>0.148990987763022</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>355</v>
       </c>
@@ -19395,7 +19399,7 @@
         <v>0.31931108115022699</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>357</v>
       </c>
@@ -19436,7 +19440,7 @@
         <v>0.31931108115022699</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>359</v>
       </c>
@@ -19477,7 +19481,7 @@
         <v>0.31931108115022699</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>374</v>
       </c>
@@ -19518,7 +19522,7 @@
         <v>0.44020960991515201</v>
       </c>
     </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>376</v>
       </c>
@@ -19559,7 +19563,7 @@
         <v>0.44020960991515201</v>
       </c>
     </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>392</v>
       </c>
@@ -19600,7 +19604,7 @@
         <v>0.58352300976369598</v>
       </c>
     </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>458</v>
       </c>
@@ -19641,7 +19645,7 @@
         <v>1.7794385315716801</v>
       </c>
     </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>476</v>
       </c>
@@ -19682,7 +19686,7 @@
         <v>2.1319704268570399</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>488</v>
       </c>
@@ -19723,7 +19727,7 @@
         <v>2.2587097587564902</v>
       </c>
     </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>512</v>
       </c>
@@ -19764,7 +19768,7 @@
         <v>2.5599108276731202</v>
       </c>
     </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>516</v>
       </c>
@@ -19805,7 +19809,7 @@
         <v>2.62675561595705</v>
       </c>
     </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>555</v>
       </c>
@@ -19846,7 +19850,7 @@
         <v>5.3096141866859003</v>
       </c>
     </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>573</v>
       </c>
@@ -19887,7 +19891,7 @@
         <v>5.5472751840980399</v>
       </c>
     </row>
-    <row r="385" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>580</v>
       </c>
@@ -19928,7 +19932,7 @@
         <v>6.0127122899324199</v>
       </c>
     </row>
-    <row r="386" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>594</v>
       </c>
@@ -19969,7 +19973,7 @@
         <v>7.29177875984489</v>
       </c>
     </row>
-    <row r="387" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>600</v>
       </c>
@@ -20010,7 +20014,7 @@
         <v>7.4409447911077304</v>
       </c>
     </row>
-    <row r="388" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>605</v>
       </c>
@@ -20051,7 +20055,7 @@
         <v>8.3003082800653001</v>
       </c>
     </row>
-    <row r="389" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>624</v>
       </c>
@@ -20092,7 +20096,7 @@
         <v>9.8367163217889804</v>
       </c>
     </row>
-    <row r="390" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>642</v>
       </c>
@@ -20133,7 +20137,7 @@
         <v>10.560912497626401</v>
       </c>
     </row>
-    <row r="391" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>654</v>
       </c>
@@ -20174,7 +20178,7 @@
         <v>12.044964406889999</v>
       </c>
     </row>
-    <row r="392" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>663</v>
       </c>
@@ -20215,7 +20219,7 @@
         <v>12.543673156213799</v>
       </c>
     </row>
-    <row r="393" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>671</v>
       </c>
@@ -20256,7 +20260,7 @@
         <v>12.547609899271199</v>
       </c>
     </row>
-    <row r="394" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>692</v>
       </c>
@@ -20297,7 +20301,7 @@
         <v>14.9634689654275</v>
       </c>
     </row>
-    <row r="395" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>707</v>
       </c>
@@ -20338,7 +20342,7 @@
         <v>15.6180985661553</v>
       </c>
     </row>
-    <row r="396" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>715</v>
       </c>
@@ -20379,7 +20383,7 @@
         <v>15.6180985661553</v>
       </c>
     </row>
-    <row r="397" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>733</v>
       </c>
@@ -20420,7 +20424,7 @@
         <v>16.649751555070701</v>
       </c>
     </row>
-    <row r="398" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>743</v>
       </c>
@@ -20461,7 +20465,7 @@
         <v>18.838194891334499</v>
       </c>
     </row>
-    <row r="399" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>745</v>
       </c>
@@ -20502,7 +20506,7 @@
         <v>18.838194891334499</v>
       </c>
     </row>
-    <row r="400" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>775</v>
       </c>
@@ -20543,7 +20547,7 @@
         <v>20.852905811953999</v>
       </c>
     </row>
-    <row r="401" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>799</v>
       </c>
@@ -20584,7 +20588,7 @@
         <v>24.738386826050402</v>
       </c>
     </row>
-    <row r="402" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>816</v>
       </c>
@@ -20625,7 +20629,7 @@
         <v>24.885383232320599</v>
       </c>
     </row>
-    <row r="403" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>817</v>
       </c>
@@ -20666,7 +20670,7 @@
         <v>24.885383232320599</v>
       </c>
     </row>
-    <row r="404" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>819</v>
       </c>
@@ -20707,7 +20711,7 @@
         <v>24.885383232320599</v>
       </c>
     </row>
-    <row r="405" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>821</v>
       </c>
@@ -20748,7 +20752,7 @@
         <v>24.885383232320599</v>
       </c>
     </row>
-    <row r="406" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>864</v>
       </c>
@@ -20789,7 +20793,7 @@
         <v>28.8450760520312</v>
       </c>
     </row>
-    <row r="407" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>866</v>
       </c>
@@ -20830,7 +20834,7 @@
         <v>28.8450760520312</v>
       </c>
     </row>
-    <row r="408" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>868</v>
       </c>
@@ -20871,7 +20875,7 @@
         <v>28.8450760520312</v>
       </c>
     </row>
-    <row r="409" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>889</v>
       </c>
@@ -20912,7 +20916,7 @@
         <v>28.8450760520312</v>
       </c>
     </row>
-    <row r="410" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>913</v>
       </c>
@@ -20953,7 +20957,7 @@
         <v>32.384481268995401</v>
       </c>
     </row>
-    <row r="411" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>915</v>
       </c>
@@ -20994,7 +20998,7 @@
         <v>32.384481268995401</v>
       </c>
     </row>
-    <row r="412" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>916</v>
       </c>
@@ -21035,7 +21039,7 @@
         <v>32.384481268995401</v>
       </c>
     </row>
-    <row r="413" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>948</v>
       </c>
@@ -21076,7 +21080,7 @@
         <v>35.695793402351804</v>
       </c>
     </row>
-    <row r="414" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>960</v>
       </c>
@@ -21117,7 +21121,7 @@
         <v>35.695793402351804</v>
       </c>
     </row>
-    <row r="415" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>961</v>
       </c>
@@ -21158,7 +21162,7 @@
         <v>35.695793402351804</v>
       </c>
     </row>
-    <row r="416" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>969</v>
       </c>
@@ -21199,7 +21203,7 @@
         <v>37.0156526138868</v>
       </c>
     </row>
-    <row r="417" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>979</v>
       </c>
@@ -21240,7 +21244,7 @@
         <v>37.1072887204148</v>
       </c>
     </row>
-    <row r="418" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>989</v>
       </c>
@@ -21281,7 +21285,7 @@
         <v>37.450789582243402</v>
       </c>
     </row>
-    <row r="419" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>991</v>
       </c>
@@ -21322,7 +21326,7 @@
         <v>37.450789582243402</v>
       </c>
     </row>
-    <row r="420" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>993</v>
       </c>
@@ -21363,7 +21367,7 @@
         <v>37.450789582243402</v>
       </c>
     </row>
-    <row r="421" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>1004</v>
       </c>
@@ -21404,7 +21408,7 @@
         <v>38.508494792924999</v>
       </c>
     </row>
-    <row r="422" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>1010</v>
       </c>
@@ -21445,7 +21449,7 @@
         <v>39.472648241525697</v>
       </c>
     </row>
-    <row r="423" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>1013</v>
       </c>
@@ -21486,7 +21490,7 @@
         <v>39.472648241525697</v>
       </c>
     </row>
-    <row r="424" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>1014</v>
       </c>
@@ -21527,7 +21531,7 @@
         <v>39.472648241525697</v>
       </c>
     </row>
-    <row r="425" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>264</v>
       </c>
@@ -21568,7 +21572,7 @@
         <v>5.5950368858555801E-3</v>
       </c>
     </row>
-    <row r="426" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>284</v>
       </c>
@@ -21609,7 +21613,7 @@
         <v>1.12404455014973E-2</v>
       </c>
     </row>
-    <row r="427" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>435</v>
       </c>
@@ -21650,7 +21654,7 @@
         <v>0.52331970230851699</v>
       </c>
     </row>
-    <row r="428" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>502</v>
       </c>
@@ -21691,7 +21695,7 @@
         <v>1.0775371354582799</v>
       </c>
     </row>
-    <row r="429" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>542</v>
       </c>
@@ -21732,7 +21736,7 @@
         <v>1.7700924299802501</v>
       </c>
     </row>
-    <row r="430" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>553</v>
       </c>
@@ -21773,7 +21777,7 @@
         <v>2.1772160752580501</v>
       </c>
     </row>
-    <row r="431" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>567</v>
       </c>
@@ -21814,7 +21818,7 @@
         <v>2.21433033791519</v>
       </c>
     </row>
-    <row r="432" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>575</v>
       </c>
@@ -21855,7 +21859,7 @@
         <v>2.21433033791519</v>
       </c>
     </row>
-    <row r="433" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>596</v>
       </c>
@@ -21896,7 +21900,7 @@
         <v>2.8910224537339499</v>
       </c>
     </row>
-    <row r="434" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>634</v>
       </c>
@@ -21937,7 +21941,7 @@
         <v>4.1527359776330703</v>
       </c>
     </row>
-    <row r="435" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>652</v>
       </c>
@@ -21978,7 +21982,7 @@
         <v>4.8855133470945598</v>
       </c>
     </row>
-    <row r="436" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>665</v>
       </c>
@@ -22019,7 +22023,7 @@
         <v>5.1627657569038599</v>
       </c>
     </row>
-    <row r="437" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>702</v>
       </c>
@@ -22060,7 +22064,7 @@
         <v>6.3348601687409696</v>
       </c>
     </row>
-    <row r="438" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>983</v>
       </c>
@@ -22101,7 +22105,7 @@
         <v>23.054520937683598</v>
       </c>
     </row>
-    <row r="439" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>985</v>
       </c>
@@ -22142,7 +22146,7 @@
         <v>23.054520937683598</v>
       </c>
     </row>
-    <row r="440" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>92</v>
       </c>
@@ -22183,7 +22187,7 @@
         <v>2.22702016235215E-9</v>
       </c>
     </row>
-    <row r="441" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>100</v>
       </c>
@@ -22224,7 +22228,7 @@
         <v>2.6499957443792999E-9</v>
       </c>
     </row>
-    <row r="442" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>109</v>
       </c>
@@ -22265,7 +22269,7 @@
         <v>5.8360361111779803E-9</v>
       </c>
     </row>
-    <row r="443" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>113</v>
       </c>
@@ -22306,7 +22310,7 @@
         <v>1.0802521899344601E-8</v>
       </c>
     </row>
-    <row r="444" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>115</v>
       </c>
@@ -22347,7 +22351,7 @@
         <v>1.1034333998648601E-8</v>
       </c>
     </row>
-    <row r="445" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>117</v>
       </c>
@@ -22388,7 +22392,7 @@
         <v>1.1034333998648601E-8</v>
       </c>
     </row>
-    <row r="446" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>118</v>
       </c>
@@ -22429,7 +22433,7 @@
         <v>1.1034333998648601E-8</v>
       </c>
     </row>
-    <row r="447" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>120</v>
       </c>
@@ -22470,7 +22474,7 @@
         <v>1.6320537461752301E-8</v>
       </c>
     </row>
-    <row r="448" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>122</v>
       </c>
@@ -22511,7 +22515,7 @@
         <v>2.77943801668825E-8</v>
       </c>
     </row>
-    <row r="449" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>123</v>
       </c>
@@ -22552,7 +22556,7 @@
         <v>3.84055443507013E-8</v>
       </c>
     </row>
-    <row r="450" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>133</v>
       </c>
@@ -22593,7 +22597,7 @@
         <v>3.5493807969312801E-7</v>
       </c>
     </row>
-    <row r="451" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>136</v>
       </c>
@@ -22634,7 +22638,7 @@
         <v>9.74147758064471E-7</v>
       </c>
     </row>
-    <row r="452" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>143</v>
       </c>
@@ -22675,7 +22679,7 @@
         <v>1.0787065472296301E-6</v>
       </c>
     </row>
-    <row r="453" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>147</v>
       </c>
@@ -22716,7 +22720,7 @@
         <v>1.3916869227433499E-6</v>
       </c>
     </row>
-    <row r="454" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>155</v>
       </c>
@@ -22757,7 +22761,7 @@
         <v>2.0748205603619699E-6</v>
       </c>
     </row>
-    <row r="455" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>157</v>
       </c>
@@ -22798,7 +22802,7 @@
         <v>2.0748205603619699E-6</v>
       </c>
     </row>
-    <row r="456" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>161</v>
       </c>
@@ -22839,7 +22843,7 @@
         <v>2.7010843749240601E-6</v>
       </c>
     </row>
-    <row r="457" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>162</v>
       </c>
@@ -22880,7 +22884,7 @@
         <v>2.7377352834658298E-6</v>
       </c>
     </row>
-    <row r="458" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>166</v>
       </c>
@@ -22921,7 +22925,7 @@
         <v>3.4649805705727102E-6</v>
       </c>
     </row>
-    <row r="459" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>170</v>
       </c>
@@ -22962,7 +22966,7 @@
         <v>4.2007114251060804E-6</v>
       </c>
     </row>
-    <row r="460" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>192</v>
       </c>
@@ -23003,7 +23007,7 @@
         <v>5.2041383064062701E-5</v>
       </c>
     </row>
-    <row r="461" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>197</v>
       </c>
@@ -23044,7 +23048,7 @@
         <v>5.9216955598107002E-5</v>
       </c>
     </row>
-    <row r="462" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>200</v>
       </c>
@@ -23085,7 +23089,7 @@
         <v>6.5977547079326904E-5</v>
       </c>
     </row>
-    <row r="463" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>201</v>
       </c>
@@ -23126,7 +23130,7 @@
         <v>8.2536229016244795E-5</v>
       </c>
     </row>
-    <row r="464" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>202</v>
       </c>
@@ -23167,7 +23171,7 @@
         <v>8.2536229016244795E-5</v>
       </c>
     </row>
-    <row r="465" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>205</v>
       </c>
@@ -23208,7 +23212,7 @@
         <v>1.71173300945861E-4</v>
       </c>
     </row>
-    <row r="466" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>212</v>
       </c>
@@ -23249,7 +23253,7 @@
         <v>2.35822191130586E-4</v>
       </c>
     </row>
-    <row r="467" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>220</v>
       </c>
@@ -23290,7 +23294,7 @@
         <v>3.3771546729721897E-4</v>
       </c>
     </row>
-    <row r="468" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>223</v>
       </c>
@@ -23331,7 +23335,7 @@
         <v>3.95227368383206E-4</v>
       </c>
     </row>
-    <row r="469" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>227</v>
       </c>
@@ -23372,7 +23376,7 @@
         <v>4.06636945821755E-4</v>
       </c>
     </row>
-    <row r="470" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>237</v>
       </c>
@@ -23413,7 +23417,7 @@
         <v>7.3467012353725203E-4</v>
       </c>
     </row>
-    <row r="471" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>239</v>
       </c>
@@ -23454,7 +23458,7 @@
         <v>7.8844852857814596E-4</v>
       </c>
     </row>
-    <row r="472" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>245</v>
       </c>
@@ -23495,7 +23499,7 @@
         <v>1.0367880688056501E-3</v>
       </c>
     </row>
-    <row r="473" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>251</v>
       </c>
@@ -23536,7 +23540,7 @@
         <v>1.4985178603592201E-3</v>
       </c>
     </row>
-    <row r="474" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>272</v>
       </c>
@@ -23577,7 +23581,7 @@
         <v>3.8537642130230402E-3</v>
       </c>
     </row>
-    <row r="475" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>304</v>
       </c>
@@ -23618,7 +23622,7 @@
         <v>1.3512816485422701E-2</v>
       </c>
     </row>
-    <row r="476" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>306</v>
       </c>
@@ -23659,7 +23663,7 @@
         <v>1.3512816485422701E-2</v>
       </c>
     </row>
-    <row r="477" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>312</v>
       </c>
@@ -23700,7 +23704,7 @@
         <v>1.4378381086047901E-2</v>
       </c>
     </row>
-    <row r="478" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>326</v>
       </c>
@@ -23741,7 +23745,7 @@
         <v>2.5607977189034101E-2</v>
       </c>
     </row>
-    <row r="479" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>336</v>
       </c>
@@ -23782,7 +23786,7 @@
         <v>3.28705204791052E-2</v>
       </c>
     </row>
-    <row r="480" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>342</v>
       </c>
@@ -23823,7 +23827,7 @@
         <v>3.8654083205751699E-2</v>
       </c>
     </row>
-    <row r="481" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>344</v>
       </c>
@@ -23864,7 +23868,7 @@
         <v>4.0032184481204401E-2</v>
       </c>
     </row>
-    <row r="482" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>346</v>
       </c>
@@ -23905,7 +23909,7 @@
         <v>4.0032184481204401E-2</v>
       </c>
     </row>
-    <row r="483" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>361</v>
       </c>
@@ -23946,7 +23950,7 @@
         <v>5.9378256079437503E-2</v>
       </c>
     </row>
-    <row r="484" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>363</v>
       </c>
@@ -23987,7 +23991,7 @@
         <v>6.1227769210375899E-2</v>
       </c>
     </row>
-    <row r="485" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>365</v>
       </c>
@@ -24028,7 +24032,7 @@
         <v>6.1227769210375899E-2</v>
       </c>
     </row>
-    <row r="486" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>366</v>
       </c>
@@ -24069,7 +24073,7 @@
         <v>6.3644511986394398E-2</v>
       </c>
     </row>
-    <row r="487" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>382</v>
       </c>
@@ -24110,7 +24114,7 @@
         <v>9.4563846050488495E-2</v>
       </c>
     </row>
-    <row r="488" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>396</v>
       </c>
@@ -24151,7 +24155,7 @@
         <v>0.117550043907256</v>
       </c>
     </row>
-    <row r="489" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>398</v>
       </c>
@@ -24192,7 +24196,7 @@
         <v>0.117550043907256</v>
       </c>
     </row>
-    <row r="490" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>400</v>
       </c>
@@ -24233,7 +24237,7 @@
         <v>0.117550043907256</v>
       </c>
     </row>
-    <row r="491" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>406</v>
       </c>
@@ -24274,7 +24278,7 @@
         <v>0.14408369471180699</v>
       </c>
     </row>
-    <row r="492" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>412</v>
       </c>
@@ -24315,7 +24319,7 @@
         <v>0.15219234707307</v>
       </c>
     </row>
-    <row r="493" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>414</v>
       </c>
@@ -24356,7 +24360,7 @@
         <v>0.15219234707307</v>
       </c>
     </row>
-    <row r="494" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>425</v>
       </c>
@@ -24397,7 +24401,7 @@
         <v>0.18263538771541701</v>
       </c>
     </row>
-    <row r="495" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>486</v>
       </c>
@@ -24438,7 +24442,7 @@
         <v>0.42352445505374398</v>
       </c>
     </row>
-    <row r="496" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>490</v>
       </c>
@@ -24479,7 +24483,7 @@
         <v>0.44339278516226199</v>
       </c>
     </row>
-    <row r="497" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>496</v>
       </c>
@@ -24520,7 +24524,7 @@
         <v>0.45752588163843699</v>
       </c>
     </row>
-    <row r="498" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>518</v>
       </c>
@@ -24561,7 +24565,7 @@
         <v>0.53700848267241796</v>
       </c>
     </row>
-    <row r="499" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>522</v>
       </c>
@@ -24602,7 +24606,7 @@
         <v>0.55159941254728795</v>
       </c>
     </row>
-    <row r="500" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>541</v>
       </c>
@@ -24643,7 +24647,7 @@
         <v>0.77735438703869897</v>
       </c>
     </row>
-    <row r="501" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>544</v>
       </c>
@@ -24684,7 +24688,7 @@
         <v>0.79570198439990403</v>
       </c>
     </row>
-    <row r="502" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>546</v>
       </c>
@@ -24725,7 +24729,7 @@
         <v>0.80941137256218698</v>
       </c>
     </row>
-    <row r="503" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>547</v>
       </c>
@@ -24766,7 +24770,7 @@
         <v>0.83681425534478504</v>
       </c>
     </row>
-    <row r="504" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>560</v>
       </c>
@@ -24807,7 +24811,7 @@
         <v>1.0303773676688399</v>
       </c>
     </row>
-    <row r="505" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>561</v>
       </c>
@@ -24848,7 +24852,7 @@
         <v>1.0303773676688399</v>
       </c>
     </row>
-    <row r="506" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>563</v>
       </c>
@@ -24889,7 +24893,7 @@
         <v>1.0303773676688399</v>
       </c>
     </row>
-    <row r="507" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>577</v>
       </c>
@@ -24930,7 +24934,7 @@
         <v>1.09726833562274</v>
       </c>
     </row>
-    <row r="508" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>579</v>
       </c>
@@ -24971,7 +24975,7 @@
         <v>1.09726833562274</v>
       </c>
     </row>
-    <row r="509" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
         <v>588</v>
       </c>
@@ -25012,7 +25016,7 @@
         <v>1.22019251604445</v>
       </c>
     </row>
-    <row r="510" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>604</v>
       </c>
@@ -25053,7 +25057,7 @@
         <v>1.68093443472772</v>
       </c>
     </row>
-    <row r="511" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>607</v>
       </c>
@@ -25094,7 +25098,7 @@
         <v>1.7326883379340201</v>
       </c>
     </row>
-    <row r="512" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>617</v>
       </c>
@@ -25135,7 +25139,7 @@
         <v>1.9827494175784499</v>
       </c>
     </row>
-    <row r="513" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>640</v>
       </c>
@@ -25176,7 +25180,7 @@
         <v>2.2685312545499099</v>
       </c>
     </row>
-    <row r="514" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>650</v>
       </c>
@@ -25217,7 +25221,7 @@
         <v>2.4872878453087202</v>
       </c>
     </row>
-    <row r="515" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>660</v>
       </c>
@@ -25258,7 +25262,7 @@
         <v>2.71497979616827</v>
       </c>
     </row>
-    <row r="516" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
         <v>662</v>
       </c>
@@ -25299,7 +25303,7 @@
         <v>2.71497979616827</v>
       </c>
     </row>
-    <row r="517" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
         <v>673</v>
       </c>
@@ -25340,7 +25344,7 @@
         <v>2.80739405247731</v>
       </c>
     </row>
-    <row r="518" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>680</v>
       </c>
@@ -25381,7 +25385,7 @@
         <v>2.8236799141178301</v>
       </c>
     </row>
-    <row r="519" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>704</v>
       </c>
@@ -25422,7 +25426,7 @@
         <v>3.5024802777355299</v>
       </c>
     </row>
-    <row r="520" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>705</v>
       </c>
@@ -25463,7 +25467,7 @@
         <v>3.5024802777355299</v>
       </c>
     </row>
-    <row r="521" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>726</v>
       </c>
@@ -25504,7 +25508,7 @@
         <v>3.6293048207440699</v>
       </c>
     </row>
-    <row r="522" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>728</v>
       </c>
@@ -25545,7 +25549,7 @@
         <v>3.6293048207440699</v>
       </c>
     </row>
-    <row r="523" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
         <v>735</v>
       </c>
@@ -25586,7 +25590,7 @@
         <v>3.8704686145463398</v>
       </c>
     </row>
-    <row r="524" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>753</v>
       </c>
@@ -25627,7 +25631,7 @@
         <v>4.7505740202344597</v>
       </c>
     </row>
-    <row r="525" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
         <v>757</v>
       </c>
@@ -25668,7 +25672,7 @@
         <v>4.7505740202344597</v>
       </c>
     </row>
-    <row r="526" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
         <v>769</v>
       </c>
@@ -25709,7 +25713,7 @@
         <v>4.8682891776422501</v>
       </c>
     </row>
-    <row r="527" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
         <v>771</v>
       </c>
@@ -25750,7 +25754,7 @@
         <v>4.8682891776422501</v>
       </c>
     </row>
-    <row r="528" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
         <v>773</v>
       </c>
@@ -25791,7 +25795,7 @@
         <v>4.8682891776422501</v>
       </c>
     </row>
-    <row r="529" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
         <v>783</v>
       </c>
@@ -25832,7 +25836,7 @@
         <v>4.9746972994028802</v>
       </c>
     </row>
-    <row r="530" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>811</v>
       </c>
@@ -25873,7 +25877,7 @@
         <v>6.1176322877385099</v>
       </c>
     </row>
-    <row r="531" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
         <v>813</v>
       </c>
@@ -25914,7 +25918,7 @@
         <v>6.1176322877385099</v>
       </c>
     </row>
-    <row r="532" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>849</v>
       </c>
@@ -25955,7 +25959,7 @@
         <v>6.8944360370197</v>
       </c>
     </row>
-    <row r="533" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>851</v>
       </c>
@@ -25996,7 +26000,7 @@
         <v>6.8944360370197</v>
       </c>
     </row>
-    <row r="534" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>859</v>
       </c>
@@ -26037,7 +26041,7 @@
         <v>7.1987731521490801</v>
       </c>
     </row>
-    <row r="535" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>870</v>
       </c>
@@ -26078,7 +26082,7 @@
         <v>7.5920403867203898</v>
       </c>
     </row>
-    <row r="536" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>901</v>
       </c>
@@ -26119,7 +26123,7 @@
         <v>8.5569623426289603</v>
       </c>
     </row>
-    <row r="537" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>902</v>
       </c>
@@ -26160,7 +26164,7 @@
         <v>8.6500057081386501</v>
       </c>
     </row>
-    <row r="538" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
         <v>911</v>
       </c>
@@ -26201,7 +26205,7 @@
         <v>8.6992788228284201</v>
       </c>
     </row>
-    <row r="539" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
         <v>946</v>
       </c>
@@ -26242,7 +26246,7 @@
         <v>9.7544867553969699</v>
       </c>
     </row>
-    <row r="540" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
         <v>971</v>
       </c>
@@ -26283,7 +26287,7 @@
         <v>10.496640624242801</v>
       </c>
     </row>
-    <row r="541" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
         <v>972</v>
       </c>
@@ -26324,7 +26328,7 @@
         <v>10.496640624242801</v>
       </c>
     </row>
-    <row r="542" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
         <v>1009</v>
       </c>
@@ -26365,7 +26369,7 @@
         <v>12.027505047122901</v>
       </c>
     </row>
-    <row r="543" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
         <v>1012</v>
       </c>
@@ -26407,6 +26411,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N543" xr:uid="{393A681D-BE2B-492E-8051-4A1EDDEC2B96}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="GOTERM_BP_DIRECT"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:N543">
     <sortCondition ref="N1"/>
   </sortState>

</xml_diff>